<commit_message>
Analysis queries with output
</commit_message>
<xml_diff>
--- a/Analysis queries with output.xlsx
+++ b/Analysis queries with output.xlsx
@@ -1,35 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babum\Desktop\CF_Data Analytics\Data Immersion\Achievement 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C4C725-D4EA-4E9E-9680-E7AFD23B315F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48D4DF73-FD5D-4D79-9CDD-E5E8D4CC6355}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Queries &amp; Output" sheetId="2" r:id="rId1"/>
     <sheet name="Analysis" sheetId="3" r:id="rId2"/>
     <sheet name="Analysis_2" sheetId="4" r:id="rId3"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Analysis!$B$20:$B$24</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Analysis!$C$19</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Analysis!$C$20:$C$24</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Analysis!$B$20:$B$24</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Analysis!$C$19</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Analysis!$C$20:$C$24</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Analysis!$B$20:$B$24</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Analysis!$C$19</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Analysis!$C$20:$C$24</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -677,22 +665,6 @@
   </si>
   <si>
     <t>rank</t>
-  </si>
-  <si>
-    <t>SELECT RANKED_GENRE .* FROM (SELECT GENRE.*,rank() OVER (PARTITION BY country ORDER BY count_genre DESC ) FROM (SELECT  F.name AS genre, J.country, COUNT (F.name) AS count_genre, SUM (D.amount) AS total_amount_paid
-FROM film A 
-INNER JOIN inventory B ON B.film_id = A.film_id
-INNER JOIN rental C ON B.inventory_id=C.inventory_id
-INNER JOIN payment D ON D.rental_id=C.rental_id
-INNER JOIN film_category E ON E.film_id = A.film_id
-INNER JOIN category F ON E.category_id = F.category_id
-INNER JOIN customer G ON C.customer_id = G.customer_id
-INNER JOIN address H ON G.address_id = H.address_id
-INNER JOIN city I ON H.city_id = I.city_id
-INNER JOIN country J ON I.country_id = J.country_id
-WHERE J.country IN ('India', 'China', 'United States', 'Japan', 'Mexico', 'Brazil','Russian Federation', 'Philippines', 'Turkey', 'Indonesia') 
-GROUP BY F.name, J.country
-ORDER BY J.country, count_genre DESC ) AS GENRE) RANKED_GENRE WHERE RANK&lt;=1;</t>
   </si>
   <si>
     <t>SELECT  C.city, D.country,COUNT(customer_id) AS customer_count
@@ -804,6 +776,29 @@
   </si>
   <si>
     <t>Top rented movies</t>
+  </si>
+  <si>
+    <t>SELECT RANKED_GENRE .* FROM (SELECT GENRE.*,rank() OVER (PARTITION BY country ORDER BY count_genre DESC ) FROM (SELECT  F.name AS genre, J.country, COUNT (F.name) AS count_genre, SUM (D.amount) AS total_amount_paid
+FROM film A 
+INNER JOIN inventory B ON B.film_id = A.film_id
+INNER JOIN rental C ON B.inventory_id=C.inventory_id
+INNER JOIN payment D ON D.rental_id=C.rental_id
+INNER JOIN film_category E ON E.film_id = A.film_id
+INNER JOIN category F ON E.category_id = F.category_id
+INNER JOIN customer G ON C.customer_id = G.customer_id
+INNER JOIN address H ON G.address_id = H.address_id
+INNER JOIN city I ON H.city_id = I.city_id
+INNER JOIN country J ON I.country_id = J.country_id
+WHERE J.country IN (SELECT D.country
+FROM customer A
+INNER JOIN address B ON A.address_id=B.address_id
+INNER JOIN city C ON B.city_id=C.city_id
+INNER JOIN country D ON C.country_id=D.country_id
+GROUP BY country
+ORDER BY COUNT(customer_id) DESC
+LIMIT 10) 
+GROUP BY F.name, J.country
+ORDER BY J.country, count_genre DESC ) AS GENRE) RANKED_GENRE WHERE RANK&lt;=1;</t>
   </si>
 </sst>
 </file>
@@ -1372,18 +1367,6 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1396,10 +1379,22 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="42" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1763,8 +1758,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView topLeftCell="A65" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1797,7 +1792,7 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="16" t="s">
         <v>58</v>
       </c>
       <c r="B3" s="4" t="s">
@@ -1850,7 +1845,7 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
+      <c r="A4" s="16"/>
       <c r="B4" s="5">
         <v>1000</v>
       </c>
@@ -1901,52 +1896,52 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
+      <c r="A5" s="16"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
+      <c r="A6" s="16"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
+      <c r="A7" s="16"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
+      <c r="A8" s="16"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="13"/>
+      <c r="A9" s="16"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
+      <c r="A10" s="16"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="13"/>
+      <c r="A11" s="16"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="13"/>
+      <c r="A12" s="16"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="13"/>
+      <c r="A13" s="16"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="13"/>
+      <c r="A14" s="16"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="13"/>
+      <c r="A15" s="16"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="13"/>
+      <c r="A16" s="16"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="13"/>
+      <c r="A17" s="16"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="13"/>
+      <c r="A18" s="16"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="13"/>
+      <c r="A19" s="16"/>
     </row>
     <row r="20" spans="1:6" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="13"/>
+      <c r="A20" s="16"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="3"/>
@@ -1960,7 +1955,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="16" t="s">
         <v>59</v>
       </c>
       <c r="B23" s="4" t="s">
@@ -1980,7 +1975,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="13"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="5">
         <v>599</v>
       </c>
@@ -1998,19 +1993,19 @@
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="13"/>
+      <c r="A25" s="16"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
+      <c r="A26" s="16"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
+      <c r="A27" s="16"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="13"/>
+      <c r="A28" s="16"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="13"/>
+      <c r="A29" s="16"/>
     </row>
     <row r="31" spans="1:6" s="7" customFormat="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="6" t="s">
@@ -2021,7 +2016,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="11" t="s">
+      <c r="A32" s="17" t="s">
         <v>64</v>
       </c>
       <c r="B32" s="4" t="s">
@@ -2032,7 +2027,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="12"/>
+      <c r="A33" s="18"/>
       <c r="B33" s="5" t="s">
         <v>46</v>
       </c>
@@ -2041,7 +2036,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="12"/>
+      <c r="A34" s="18"/>
       <c r="B34" s="5" t="s">
         <v>48</v>
       </c>
@@ -2050,7 +2045,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="12"/>
+      <c r="A35" s="18"/>
       <c r="B35" s="5" t="s">
         <v>42</v>
       </c>
@@ -2059,7 +2054,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="12"/>
+      <c r="A36" s="18"/>
       <c r="B36" s="5" t="s">
         <v>49</v>
       </c>
@@ -2068,7 +2063,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="12"/>
+      <c r="A37" s="18"/>
       <c r="B37" s="5" t="s">
         <v>31</v>
       </c>
@@ -2077,7 +2072,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="12"/>
+      <c r="A38" s="18"/>
       <c r="B38" s="5" t="s">
         <v>50</v>
       </c>
@@ -2086,7 +2081,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="12"/>
+      <c r="A39" s="18"/>
       <c r="B39" s="5" t="s">
         <v>51</v>
       </c>
@@ -2095,7 +2090,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="12"/>
+      <c r="A40" s="18"/>
       <c r="B40" s="5" t="s">
         <v>52</v>
       </c>
@@ -2104,7 +2099,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
+      <c r="A41" s="18"/>
       <c r="B41" s="5" t="s">
         <v>35</v>
       </c>
@@ -2113,7 +2108,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="12"/>
+      <c r="A42" s="18"/>
       <c r="B42" s="5" t="s">
         <v>53</v>
       </c>
@@ -2124,15 +2119,15 @@
     <row r="43" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="45" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
-        <v>182</v>
+      <c r="A46" s="16" t="s">
+        <v>181</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>25</v>
@@ -2145,7 +2140,7 @@
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="13"/>
+      <c r="A47" s="16"/>
       <c r="B47" s="5" t="s">
         <v>41</v>
       </c>
@@ -2157,7 +2152,7 @@
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="13"/>
+      <c r="A48" s="16"/>
       <c r="B48" s="5" t="s">
         <v>30</v>
       </c>
@@ -2169,7 +2164,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="13"/>
+      <c r="A49" s="16"/>
       <c r="B49" s="5" t="s">
         <v>57</v>
       </c>
@@ -2181,7 +2176,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="13"/>
+      <c r="A50" s="16"/>
       <c r="B50" s="5" t="s">
         <v>45</v>
       </c>
@@ -2193,7 +2188,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="13"/>
+      <c r="A51" s="16"/>
       <c r="B51" s="5" t="s">
         <v>55</v>
       </c>
@@ -2205,7 +2200,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="13"/>
+      <c r="A52" s="16"/>
       <c r="B52" s="5" t="s">
         <v>56</v>
       </c>
@@ -2217,7 +2212,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
+      <c r="A53" s="16"/>
       <c r="B53" s="5" t="s">
         <v>54</v>
       </c>
@@ -2229,7 +2224,7 @@
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
+      <c r="A54" s="16"/>
       <c r="B54" s="5" t="s">
         <v>34</v>
       </c>
@@ -2241,7 +2236,7 @@
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
+      <c r="A55" s="16"/>
       <c r="B55" s="5" t="s">
         <v>38</v>
       </c>
@@ -2253,9 +2248,9 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
+      <c r="A56" s="16"/>
       <c r="B56" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>50</v>
@@ -2265,34 +2260,34 @@
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
+      <c r="A57" s="16"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" s="13"/>
+      <c r="A58" s="16"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="13"/>
+      <c r="A59" s="16"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="13"/>
+      <c r="A60" s="16"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="13"/>
+      <c r="A61" s="16"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="13"/>
+      <c r="A62" s="16"/>
     </row>
     <row r="64" spans="1:4" ht="37.5" x14ac:dyDescent="0.3">
       <c r="A64" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="13" t="s">
-        <v>185</v>
+      <c r="A65" s="16" t="s">
+        <v>184</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>22</v>
@@ -2314,7 +2309,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
+      <c r="A66" s="16"/>
       <c r="B66" s="5">
         <v>84</v>
       </c>
@@ -2335,7 +2330,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
+      <c r="A67" s="16"/>
       <c r="B67" s="5">
         <v>518</v>
       </c>
@@ -2356,7 +2351,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
+      <c r="A68" s="16"/>
       <c r="B68" s="5">
         <v>587</v>
       </c>
@@ -2377,7 +2372,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
+      <c r="A69" s="16"/>
       <c r="B69" s="5">
         <v>537</v>
       </c>
@@ -2398,7 +2393,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
+      <c r="A70" s="16"/>
       <c r="B70" s="5">
         <v>367</v>
       </c>
@@ -2419,73 +2414,73 @@
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
+      <c r="A71" s="16"/>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
+      <c r="A72" s="16"/>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="13"/>
+      <c r="A73" s="16"/>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A74" s="13"/>
+      <c r="A74" s="16"/>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="13"/>
+      <c r="A75" s="16"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="13"/>
+      <c r="A76" s="16"/>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="13"/>
+      <c r="A77" s="16"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="13"/>
+      <c r="A78" s="16"/>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="13"/>
+      <c r="A79" s="16"/>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="13"/>
+      <c r="A80" s="16"/>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="13"/>
+      <c r="A81" s="16"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="13"/>
+      <c r="A82" s="16"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="13"/>
+      <c r="A83" s="16"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="13"/>
+      <c r="A84" s="16"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="13"/>
+      <c r="A85" s="16"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="13"/>
+      <c r="A86" s="16"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="13"/>
+      <c r="A87" s="16"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="13"/>
+      <c r="A88" s="16"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="13"/>
+      <c r="A89" s="16"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="13"/>
+      <c r="A90" s="16"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="13"/>
+      <c r="A91" s="16"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="13"/>
+      <c r="A92" s="16"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="13"/>
+      <c r="A93" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -2518,7 +2513,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="13" t="s">
         <v>101</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -2526,7 +2521,7 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="19" t="s">
         <v>63</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2534,7 +2529,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="14"/>
+      <c r="A3" s="19"/>
       <c r="B3" s="5">
         <v>61312.04</v>
       </c>
@@ -2548,7 +2543,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="19" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -2571,7 +2566,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="5">
         <v>148</v>
       </c>
@@ -2592,7 +2587,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="5">
         <v>526</v>
       </c>
@@ -2613,7 +2608,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="5">
         <v>178</v>
       </c>
@@ -2634,7 +2629,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="5">
         <v>137</v>
       </c>
@@ -2655,7 +2650,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="5">
         <v>144</v>
       </c>
@@ -2676,7 +2671,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="5">
         <v>459</v>
       </c>
@@ -2697,7 +2692,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="5">
         <v>181</v>
       </c>
@@ -2718,7 +2713,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="5">
         <v>410</v>
       </c>
@@ -2739,7 +2734,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="5">
         <v>236</v>
       </c>
@@ -2760,7 +2755,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="5">
         <v>403</v>
       </c>
@@ -2789,7 +2784,7 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="14" t="s">
+      <c r="A19" s="19" t="s">
         <v>127</v>
       </c>
       <c r="B19" s="4" t="s">
@@ -2800,7 +2795,7 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="5" t="s">
         <v>20</v>
       </c>
@@ -2809,7 +2804,7 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="5" t="s">
         <v>107</v>
       </c>
@@ -2818,7 +2813,7 @@
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="5" t="s">
         <v>105</v>
       </c>
@@ -2827,7 +2822,7 @@
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="19"/>
       <c r="B23" s="5" t="s">
         <v>126</v>
       </c>
@@ -2836,7 +2831,7 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="5" t="s">
         <v>112</v>
       </c>
@@ -2845,12 +2840,12 @@
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
     </row>
     <row r="27" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="13" t="s">
         <v>130</v>
       </c>
       <c r="B27" s="7" t="s">
@@ -2858,24 +2853,24 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="14" t="s">
+      <c r="A28" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C28" s="15" t="s">
+      <c r="C28" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
+      <c r="A29" s="19"/>
       <c r="B29" s="5" t="s">
         <v>104</v>
       </c>
@@ -2890,7 +2885,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="14"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="5" t="s">
         <v>106</v>
       </c>
@@ -2905,7 +2900,7 @@
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="14"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="5" t="s">
         <v>108</v>
       </c>
@@ -2920,7 +2915,7 @@
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="14"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="5" t="s">
         <v>109</v>
       </c>
@@ -2935,7 +2930,7 @@
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="14"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="5" t="s">
         <v>110</v>
       </c>
@@ -2950,7 +2945,7 @@
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="14"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="5" t="s">
         <v>111</v>
       </c>
@@ -2965,7 +2960,7 @@
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="14"/>
+      <c r="A35" s="19"/>
       <c r="B35" s="5" t="s">
         <v>113</v>
       </c>
@@ -2980,7 +2975,7 @@
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="14"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="5" t="s">
         <v>114</v>
       </c>
@@ -2995,7 +2990,7 @@
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="14"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="5" t="s">
         <v>115</v>
       </c>
@@ -3010,7 +3005,7 @@
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="14"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="5" t="s">
         <v>116</v>
       </c>
@@ -3025,7 +3020,7 @@
       </c>
     </row>
     <row r="40" spans="1:5" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="13" t="s">
         <v>144</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -3033,24 +3028,24 @@
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="11" t="s">
         <v>102</v>
       </c>
-      <c r="C41" s="15" t="s">
+      <c r="C41" s="11" t="s">
         <v>103</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="14"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="5" t="s">
         <v>119</v>
       </c>
@@ -3065,7 +3060,7 @@
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="14"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="5" t="s">
         <v>118</v>
       </c>
@@ -3080,7 +3075,7 @@
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="14"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="5" t="s">
         <v>117</v>
       </c>
@@ -3095,7 +3090,7 @@
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="14"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="5" t="s">
         <v>120</v>
       </c>
@@ -3110,7 +3105,7 @@
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="14"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="5" t="s">
         <v>122</v>
       </c>
@@ -3125,7 +3120,7 @@
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="14"/>
+      <c r="A47" s="19"/>
       <c r="B47" s="5" t="s">
         <v>121</v>
       </c>
@@ -3140,7 +3135,7 @@
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="14"/>
+      <c r="A48" s="19"/>
       <c r="B48" s="5" t="s">
         <v>123</v>
       </c>
@@ -3155,7 +3150,7 @@
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="14"/>
+      <c r="A49" s="19"/>
       <c r="B49" s="5" t="s">
         <v>124</v>
       </c>
@@ -3170,7 +3165,7 @@
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="14"/>
+      <c r="A50" s="19"/>
       <c r="B50" s="5" t="s">
         <v>125</v>
       </c>
@@ -3185,7 +3180,7 @@
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="14"/>
+      <c r="A51" s="19"/>
       <c r="B51" s="5" t="s">
         <v>143</v>
       </c>
@@ -3208,7 +3203,7 @@
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="14" t="s">
+      <c r="A54" s="19" t="s">
         <v>146</v>
       </c>
       <c r="B54" s="4" t="s">
@@ -3222,7 +3217,7 @@
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="14"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="5" t="s">
         <v>46</v>
       </c>
@@ -3232,10 +3227,10 @@
       <c r="D55" s="5">
         <v>6034.78</v>
       </c>
-      <c r="E55" s="20"/>
+      <c r="E55" s="15"/>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="14"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="5" t="s">
         <v>48</v>
       </c>
@@ -3245,10 +3240,10 @@
       <c r="D56" s="5">
         <v>5251.03</v>
       </c>
-      <c r="E56" s="20"/>
+      <c r="E56" s="15"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="14"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="5" t="s">
         <v>42</v>
       </c>
@@ -3258,10 +3253,10 @@
       <c r="D57" s="5">
         <v>3685.31</v>
       </c>
-      <c r="E57" s="20"/>
+      <c r="E57" s="15"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="14"/>
+      <c r="A58" s="19"/>
       <c r="B58" s="5" t="s">
         <v>49</v>
       </c>
@@ -3271,10 +3266,10 @@
       <c r="D58" s="5">
         <v>3122.51</v>
       </c>
-      <c r="E58" s="20"/>
+      <c r="E58" s="15"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" s="14"/>
+      <c r="A59" s="19"/>
       <c r="B59" s="5" t="s">
         <v>31</v>
       </c>
@@ -3284,10 +3279,10 @@
       <c r="D59" s="5">
         <v>2984.82</v>
       </c>
-      <c r="E59" s="20"/>
+      <c r="E59" s="15"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" s="14"/>
+      <c r="A60" s="19"/>
       <c r="B60" s="5" t="s">
         <v>50</v>
       </c>
@@ -3297,10 +3292,10 @@
       <c r="D60" s="5">
         <v>2919.19</v>
       </c>
-      <c r="E60" s="20"/>
+      <c r="E60" s="15"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A61" s="14"/>
+      <c r="A61" s="19"/>
       <c r="B61" s="5" t="s">
         <v>51</v>
       </c>
@@ -3310,10 +3305,10 @@
       <c r="D61" s="5">
         <v>2765.62</v>
       </c>
-      <c r="E61" s="20"/>
+      <c r="E61" s="15"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A62" s="14"/>
+      <c r="A62" s="19"/>
       <c r="B62" s="5" t="s">
         <v>52</v>
       </c>
@@ -3323,10 +3318,10 @@
       <c r="D62" s="5">
         <v>2219.6999999999998</v>
       </c>
-      <c r="E62" s="20"/>
+      <c r="E62" s="15"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A63" s="14"/>
+      <c r="A63" s="19"/>
       <c r="B63" s="5" t="s">
         <v>35</v>
       </c>
@@ -3336,10 +3331,10 @@
       <c r="D63" s="5">
         <v>1498.49</v>
       </c>
-      <c r="E63" s="20"/>
+      <c r="E63" s="15"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A64" s="14"/>
+      <c r="A64" s="19"/>
       <c r="B64" s="5" t="s">
         <v>53</v>
       </c>
@@ -3349,7 +3344,7 @@
       <c r="D64" s="5">
         <v>1352.69</v>
       </c>
-      <c r="E64" s="20"/>
+      <c r="E64" s="15"/>
     </row>
     <row r="66" spans="1:6" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A66" s="9" t="s">
@@ -3360,7 +3355,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A67" s="14" t="s">
+      <c r="A67" s="19" t="s">
         <v>148</v>
       </c>
       <c r="B67" s="4" t="s">
@@ -3374,7 +3369,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" s="14"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="5" t="s">
         <v>149</v>
       </c>
@@ -3384,10 +3379,10 @@
       <c r="D68" s="5">
         <v>47.85</v>
       </c>
-      <c r="E68" s="20"/>
+      <c r="E68" s="15"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A69" s="14"/>
+      <c r="A69" s="19"/>
       <c r="B69" s="5" t="s">
         <v>150</v>
       </c>
@@ -3397,10 +3392,10 @@
       <c r="D69" s="5">
         <v>63.78</v>
       </c>
-      <c r="E69" s="20"/>
+      <c r="E69" s="15"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" s="14"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="5" t="s">
         <v>151</v>
       </c>
@@ -3410,10 +3405,10 @@
       <c r="D70" s="5">
         <v>64.819999999999993</v>
       </c>
-      <c r="E70" s="20"/>
+      <c r="E70" s="15"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" s="14"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="5" t="s">
         <v>152</v>
       </c>
@@ -3423,10 +3418,10 @@
       <c r="D71" s="5">
         <v>64.84</v>
       </c>
-      <c r="E71" s="20"/>
+      <c r="E71" s="15"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" s="14"/>
+      <c r="A72" s="19"/>
       <c r="B72" s="5" t="s">
         <v>153</v>
       </c>
@@ -3436,10 +3431,10 @@
       <c r="D72" s="5">
         <v>67.819999999999993</v>
       </c>
-      <c r="E72" s="20"/>
+      <c r="E72" s="15"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A73" s="14"/>
+      <c r="A73" s="19"/>
       <c r="B73" s="5" t="s">
         <v>154</v>
       </c>
@@ -3449,10 +3444,10 @@
       <c r="D73" s="5">
         <v>73.78</v>
       </c>
-      <c r="E73" s="20"/>
+      <c r="E73" s="15"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A74" s="14"/>
+      <c r="A74" s="19"/>
       <c r="B74" s="5" t="s">
         <v>155</v>
       </c>
@@ -3462,10 +3457,10 @@
       <c r="D74" s="5">
         <v>78.790000000000006</v>
       </c>
-      <c r="E74" s="20"/>
+      <c r="E74" s="15"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="19"/>
       <c r="B75" s="5" t="s">
         <v>156</v>
       </c>
@@ -3475,10 +3470,10 @@
       <c r="D75" s="5">
         <v>80.77</v>
       </c>
-      <c r="E75" s="20"/>
+      <c r="E75" s="15"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="19"/>
       <c r="B76" s="5" t="s">
         <v>157</v>
       </c>
@@ -3488,10 +3483,10 @@
       <c r="D76" s="5">
         <v>85.77</v>
       </c>
-      <c r="E76" s="20"/>
+      <c r="E76" s="15"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="19"/>
       <c r="B77" s="5" t="s">
         <v>158</v>
       </c>
@@ -3501,10 +3496,10 @@
       <c r="D77" s="5">
         <v>91.77</v>
       </c>
-      <c r="E77" s="20"/>
+      <c r="E77" s="15"/>
     </row>
     <row r="79" spans="1:6" s="2" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A79" s="17" t="s">
+      <c r="A79" s="13" t="s">
         <v>167</v>
       </c>
       <c r="B79" s="7" t="s">
@@ -3512,7 +3507,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" s="14" t="s">
+      <c r="A80" s="19" t="s">
         <v>175</v>
       </c>
       <c r="B80" s="4" t="s">
@@ -3532,7 +3527,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" s="14"/>
+      <c r="A81" s="19"/>
       <c r="B81" s="5">
         <v>2</v>
       </c>
@@ -3550,7 +3545,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" s="14"/>
+      <c r="A82" s="19"/>
       <c r="B82" s="5">
         <v>1</v>
       </c>
@@ -3568,7 +3563,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" s="14"/>
+      <c r="A83" s="19"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
@@ -3576,7 +3571,7 @@
       <c r="F83" s="5"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" s="14"/>
+      <c r="A84" s="19"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
@@ -3584,7 +3579,7 @@
       <c r="F84" s="5"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" s="14"/>
+      <c r="A85" s="19"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
@@ -3592,7 +3587,7 @@
       <c r="F85" s="5"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" s="14"/>
+      <c r="A86" s="19"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
@@ -3600,7 +3595,7 @@
       <c r="F86" s="5"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" s="14"/>
+      <c r="A87" s="19"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
@@ -3608,7 +3603,7 @@
       <c r="F87" s="5"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" s="14"/>
+      <c r="A88" s="19"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
@@ -3616,7 +3611,7 @@
       <c r="F88" s="5"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A89" s="14"/>
+      <c r="A89" s="19"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
@@ -3632,27 +3627,27 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" s="14" t="s">
+      <c r="A92" s="19" t="s">
         <v>176</v>
       </c>
-      <c r="B92" s="15" t="s">
+      <c r="B92" s="11" t="s">
         <v>131</v>
       </c>
-      <c r="C92" s="15" t="s">
+      <c r="C92" s="11" t="s">
         <v>177</v>
       </c>
-      <c r="D92" s="15" t="s">
+      <c r="D92" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="E92" s="15" t="s">
+      <c r="E92" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="F92" s="15" t="s">
+      <c r="F92" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" s="14"/>
+      <c r="A93" s="19"/>
       <c r="B93" s="5" t="s">
         <v>136</v>
       </c>
@@ -3670,7 +3665,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" s="14"/>
+      <c r="A94" s="19"/>
       <c r="B94" s="5" t="s">
         <v>137</v>
       </c>
@@ -3688,7 +3683,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" s="14"/>
+      <c r="A95" s="19"/>
       <c r="B95" s="5" t="s">
         <v>139</v>
       </c>
@@ -3706,7 +3701,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" s="14"/>
+      <c r="A96" s="19"/>
       <c r="B96" s="5" t="s">
         <v>138</v>
       </c>
@@ -3724,7 +3719,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A97" s="14"/>
+      <c r="A97" s="19"/>
       <c r="B97" s="5" t="s">
         <v>133</v>
       </c>
@@ -3742,7 +3737,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A98" s="14"/>
+      <c r="A98" s="19"/>
       <c r="B98" s="5" t="s">
         <v>140</v>
       </c>
@@ -3760,7 +3755,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A99" s="14"/>
+      <c r="A99" s="19"/>
       <c r="B99" s="5" t="s">
         <v>159</v>
       </c>
@@ -3778,7 +3773,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="14"/>
+      <c r="A100" s="19"/>
       <c r="B100" s="5" t="s">
         <v>135</v>
       </c>
@@ -3796,7 +3791,7 @@
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A101" s="14"/>
+      <c r="A101" s="19"/>
       <c r="B101" s="5" t="s">
         <v>160</v>
       </c>
@@ -3814,7 +3809,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A102" s="14"/>
+      <c r="A102" s="19"/>
       <c r="B102" s="5" t="s">
         <v>161</v>
       </c>
@@ -3832,7 +3827,7 @@
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A103" s="14"/>
+      <c r="A103" s="19"/>
       <c r="B103" s="5" t="s">
         <v>134</v>
       </c>
@@ -3850,7 +3845,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="14"/>
+      <c r="A104" s="19"/>
       <c r="B104" s="5" t="s">
         <v>141</v>
       </c>
@@ -3868,7 +3863,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="14"/>
+      <c r="A105" s="19"/>
       <c r="B105" s="5" t="s">
         <v>142</v>
       </c>
@@ -3886,7 +3881,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="14"/>
+      <c r="A106" s="19"/>
       <c r="B106" s="5" t="s">
         <v>162</v>
       </c>
@@ -3904,7 +3899,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A107" s="14"/>
+      <c r="A107" s="19"/>
       <c r="B107" s="5" t="s">
         <v>163</v>
       </c>
@@ -3922,7 +3917,7 @@
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A108" s="14"/>
+      <c r="A108" s="19"/>
       <c r="B108" s="5" t="s">
         <v>132</v>
       </c>
@@ -3940,7 +3935,7 @@
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A109" s="14"/>
+      <c r="A109" s="19"/>
       <c r="B109" s="5" t="s">
         <v>164</v>
       </c>
@@ -3958,16 +3953,16 @@
       </c>
     </row>
     <row r="111" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A111" s="18" t="s">
-        <v>201</v>
-      </c>
-      <c r="B111" s="16" t="s">
+      <c r="A111" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="B111" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A112" s="14" t="s">
-        <v>200</v>
+      <c r="A112" s="19" t="s">
+        <v>199</v>
       </c>
       <c r="B112" s="4" t="s">
         <v>102</v>
@@ -3979,19 +3974,19 @@
         <v>131</v>
       </c>
       <c r="E112" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F112" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="F112" s="4" t="s">
-        <v>190</v>
       </c>
       <c r="G112" s="4" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A113" s="14"/>
+      <c r="A113" s="19"/>
       <c r="B113" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C113" s="5" t="s">
         <v>20</v>
@@ -4010,9 +4005,9 @@
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A114" s="14"/>
+      <c r="A114" s="19"/>
       <c r="B114" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C114" s="5" t="s">
         <v>20</v>
@@ -4031,9 +4026,9 @@
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="14"/>
+      <c r="A115" s="19"/>
       <c r="B115" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C115" s="5" t="s">
         <v>107</v>
@@ -4052,9 +4047,9 @@
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A116" s="14"/>
+      <c r="A116" s="19"/>
       <c r="B116" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C116" s="5" t="s">
         <v>20</v>
@@ -4073,9 +4068,9 @@
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A117" s="14"/>
+      <c r="A117" s="19"/>
       <c r="B117" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C117" s="5" t="s">
         <v>20</v>
@@ -4094,9 +4089,9 @@
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A118" s="14"/>
+      <c r="A118" s="19"/>
       <c r="B118" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C118" s="5" t="s">
         <v>105</v>
@@ -4115,9 +4110,9 @@
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A119" s="14"/>
+      <c r="A119" s="19"/>
       <c r="B119" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C119" s="5" t="s">
         <v>105</v>
@@ -4136,9 +4131,9 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="14"/>
+      <c r="A120" s="19"/>
       <c r="B120" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C120" s="5" t="s">
         <v>20</v>
@@ -4157,9 +4152,9 @@
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A121" s="14"/>
+      <c r="A121" s="19"/>
       <c r="B121" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C121" s="5" t="s">
         <v>105</v>
@@ -4178,7 +4173,7 @@
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A122" s="14"/>
+      <c r="A122" s="19"/>
       <c r="B122" s="5" t="s">
         <v>116</v>
       </c>
@@ -4220,8 +4215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:L33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4239,22 +4234,22 @@
   <sheetData>
     <row r="2" spans="1:12" s="7" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="19" t="s">
-        <v>187</v>
-      </c>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
+      <c r="H2" s="20" t="s">
+        <v>186</v>
+      </c>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="14" t="s">
-        <v>181</v>
+      <c r="A3" s="19" t="s">
+        <v>201</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>131</v>
@@ -4288,7 +4283,7 @@
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A4" s="14"/>
+      <c r="A4" s="19"/>
       <c r="B4" s="5" t="s">
         <v>137</v>
       </c>
@@ -4321,7 +4316,7 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="14"/>
+      <c r="A5" s="19"/>
       <c r="B5" s="5" t="s">
         <v>139</v>
       </c>
@@ -4354,7 +4349,7 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="5" t="s">
         <v>134</v>
       </c>
@@ -4387,7 +4382,7 @@
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A7" s="14"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="5" t="s">
         <v>159</v>
       </c>
@@ -4420,7 +4415,7 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="14"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="5" t="s">
         <v>139</v>
       </c>
@@ -4453,7 +4448,7 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="14"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="5" t="s">
         <v>136</v>
       </c>
@@ -4486,7 +4481,7 @@
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A10" s="14"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="5" t="s">
         <v>139</v>
       </c>
@@ -4519,7 +4514,7 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="14"/>
+      <c r="A11" s="19"/>
       <c r="B11" s="5" t="s">
         <v>161</v>
       </c>
@@ -4552,7 +4547,7 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="14"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="5" t="s">
         <v>138</v>
       </c>
@@ -4585,7 +4580,7 @@
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A13" s="14"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="5" t="s">
         <v>159</v>
       </c>
@@ -4618,7 +4613,7 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="14"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="5" t="s">
         <v>136</v>
       </c>
@@ -4651,7 +4646,7 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="14"/>
+      <c r="A15" s="19"/>
       <c r="H15" s="5" t="s">
         <v>138</v>
       </c>
@@ -4669,7 +4664,7 @@
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="14"/>
+      <c r="A16" s="19"/>
       <c r="H16" s="5" t="s">
         <v>139</v>
       </c>
@@ -4687,7 +4682,7 @@
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A17" s="14"/>
+      <c r="A17" s="19"/>
       <c r="H17" s="5" t="s">
         <v>140</v>
       </c>
@@ -4705,7 +4700,7 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="14"/>
+      <c r="A18" s="19"/>
       <c r="H18" s="5" t="s">
         <v>137</v>
       </c>
@@ -4723,7 +4718,7 @@
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A19" s="14"/>
+      <c r="A19" s="19"/>
       <c r="H19" s="5" t="s">
         <v>136</v>
       </c>
@@ -4741,7 +4736,7 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="14"/>
+      <c r="A20" s="19"/>
       <c r="H20" s="5" t="s">
         <v>137</v>
       </c>
@@ -4759,7 +4754,7 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="14"/>
+      <c r="A21" s="19"/>
       <c r="H21" s="5" t="s">
         <v>135</v>
       </c>
@@ -4777,7 +4772,7 @@
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" s="14"/>
+      <c r="A22" s="19"/>
       <c r="H22" s="5" t="s">
         <v>139</v>
       </c>
@@ -4795,7 +4790,7 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="14"/>
+      <c r="A23" s="19"/>
       <c r="H23" s="5" t="s">
         <v>135</v>
       </c>
@@ -4813,7 +4808,7 @@
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A24" s="14"/>
+      <c r="A24" s="19"/>
       <c r="H24" s="5" t="s">
         <v>136</v>
       </c>
@@ -4831,7 +4826,7 @@
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A25" s="14"/>
+      <c r="A25" s="19"/>
       <c r="H25" s="5" t="s">
         <v>161</v>
       </c>
@@ -4849,7 +4844,7 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="14"/>
+      <c r="A26" s="19"/>
       <c r="H26" s="5" t="s">
         <v>139</v>
       </c>

</xml_diff>